<commit_message>
original excel for testcase
</commit_message>
<xml_diff>
--- a/auto_UI/testcase/data/test_login.xlsx
+++ b/auto_UI/testcase/data/test_login.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2775" windowWidth="19590" windowHeight="4470"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>username</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -65,26 +65,6 @@
   </si>
   <si>
     <t>caseid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>验证码输入错误，请重新输入。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pass</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>验证码输入错误，请重新输入。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fail</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>验证码输入错误，请重新输入。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -109,24 +89,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -143,14 +111,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -450,7 +415,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -479,24 +444,20 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1">
@@ -507,12 +468,8 @@
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1">
@@ -527,12 +484,8 @@
       <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1">
@@ -545,12 +498,8 @@
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>